<commit_message>
Feedback function continued development
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847C4B07-A6A2-47EE-AF19-F93675C56B77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F6AD34-446A-484C-9A75-4FAF1BD0E95A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="31140" yWindow="495" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -98,13 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,20 +382,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.9296875" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -409,7 +406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -417,17 +414,6 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
-        <v>296227</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continuation of customer feedback test development
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F6AD34-446A-484C-9A75-4FAF1BD0E95A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7BC93F-A4BC-49CD-8B1D-98C7A7B01262}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="31140" yWindow="495" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>YE_Feedback_Knowledge</t>
+  </si>
+  <si>
+    <t>Agreed_price</t>
+  </si>
+  <si>
+    <t>YE_Estimate</t>
   </si>
 </sst>
 </file>
@@ -382,20 +391,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -405,8 +416,14 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -414,6 +431,12 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continuation of the E2E customer feedback function and validation
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7BC93F-A4BC-49CD-8B1D-98C7A7B01262}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D3F80C-44F9-4DFD-8BAB-6BB51094C246}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>YE_Estimate</t>
+  </si>
+  <si>
+    <t>member for</t>
+  </si>
+  <si>
+    <t>Account_Membership_Term</t>
   </si>
 </sst>
 </file>
@@ -391,22 +397,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="2" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -414,29 +420,35 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit of "Give Feedback" after 1st clean E2E run, need to parameterize and Robustitube
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D3F80C-44F9-4DFD-8BAB-6BB51094C246}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D850AAFE-616F-409C-BB7B-64BB452272DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32040" yWindow="1800" windowWidth="20310" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -58,13 +58,175 @@
   </si>
   <si>
     <t>Account_Membership_Term</t>
+  </si>
+  <si>
+    <t>YS_Tidiness</t>
+  </si>
+  <si>
+    <t>YS_Courtesy</t>
+  </si>
+  <si>
+    <t>YS_Reliability</t>
+  </si>
+  <si>
+    <t>YS_Workmanship</t>
+  </si>
+  <si>
+    <t>YS_Work_Description</t>
+  </si>
+  <si>
+    <t>New Test Toilet</t>
+  </si>
+  <si>
+    <t>YS_Work_Date</t>
+  </si>
+  <si>
+    <t>YS_Days_to_CompleteYS_Work_Comments</t>
+  </si>
+  <si>
+    <t>YS_Feedback_Published</t>
+  </si>
+  <si>
+    <t>Nice job</t>
+  </si>
+  <si>
+    <t>YD_Consumer_Customer</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>YD_Salutation</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>YD_Name</t>
+  </si>
+  <si>
+    <t>Ron Smith</t>
+  </si>
+  <si>
+    <t>YD_Postcode</t>
+  </si>
+  <si>
+    <t>YD_Verify_Address</t>
+  </si>
+  <si>
+    <t>YD_Best_Contact_Time</t>
+  </si>
+  <si>
+    <t>YD_Email</t>
+  </si>
+  <si>
+    <t>YD_Mobile</t>
+  </si>
+  <si>
+    <t>YD_Feedback_Method</t>
+  </si>
+  <si>
+    <t>YD_How_Did_You_Hear</t>
+  </si>
+  <si>
+    <t>YD_Reason_For_Tradeperson_Selection</t>
+  </si>
+  <si>
+    <t>YD_Receive_Chekatrade_Updates</t>
+  </si>
+  <si>
+    <t>YD_Receive_Third_Party_Updates</t>
+  </si>
+  <si>
+    <t>PO12 2SD</t>
+  </si>
+  <si>
+    <t>26 Broadsands Drive,Gosport,Hampshire,PO12:</t>
+  </si>
+  <si>
+    <t>Any Tme</t>
+  </si>
+  <si>
+    <t>burt_millichip@amail.com</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>YD_Company_Name</t>
+  </si>
+  <si>
+    <t>Testing Ltd</t>
+  </si>
+  <si>
+    <t>YD_Other_Response</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Had a dream</t>
+  </si>
+  <si>
+    <t>Prefer not to say</t>
+  </si>
+  <si>
+    <t>FD_Value_of_Work</t>
+  </si>
+  <si>
+    <t>FD_Verify_Sub_Header</t>
+  </si>
+  <si>
+    <t>FD_Verify_Button_Text</t>
+  </si>
+  <si>
+    <t>Value Of Work</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>FD_Sub_Text</t>
+  </si>
+  <si>
+    <t>Data Protection Act</t>
+  </si>
+  <si>
+    <t>FP_Sub_Header_Verify</t>
+  </si>
+  <si>
+    <t>FP_Sub_Text</t>
+  </si>
+  <si>
+    <t>FP_Button_Text</t>
+  </si>
+  <si>
+    <t>HP_Header_Verification</t>
+  </si>
+  <si>
+    <t>HP_Member_Link_Text_Verification</t>
+  </si>
+  <si>
+    <t>Thank you!</t>
+  </si>
+  <si>
+    <t>A Checkatrade staff member will now review</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Helping you find the right trade or service</t>
+  </si>
+  <si>
+    <t>or look up a member by name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +247,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -110,15 +280,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,22 +573,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
+    <col min="21" max="21" width="43.42578125" customWidth="1"/>
+    <col min="22" max="22" width="21.28515625" customWidth="1"/>
+    <col min="23" max="23" width="25" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" customWidth="1"/>
+    <col min="25" max="25" width="21.85546875" customWidth="1"/>
+    <col min="26" max="27" width="22.140625" customWidth="1"/>
+    <col min="28" max="28" width="36.5703125" customWidth="1"/>
+    <col min="29" max="29" width="30.85546875" customWidth="1"/>
+    <col min="30" max="30" width="31" customWidth="1"/>
+    <col min="31" max="31" width="18.5703125" customWidth="1"/>
+    <col min="32" max="32" width="22.140625" customWidth="1"/>
+    <col min="33" max="33" width="21.5703125" customWidth="1"/>
+    <col min="34" max="34" width="18" customWidth="1"/>
+    <col min="35" max="35" width="29.28515625" customWidth="1"/>
+    <col min="36" max="36" width="34.140625" customWidth="1"/>
+    <col min="37" max="37" width="17.28515625" customWidth="1"/>
+    <col min="38" max="38" width="37.7109375" customWidth="1"/>
+    <col min="39" max="39" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -431,8 +640,104 @@
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -451,9 +756,108 @@
       <c r="F2" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="3">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="3">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2">
+        <v>7788123456</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="W2" r:id="rId1" xr:uid="{2704FD4B-CF14-4148-BC2D-3E290DE31A7D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parameterising of Feedback test function
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D850AAFE-616F-409C-BB7B-64BB452272DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0AD300-6519-409A-9D25-20D0A3DC15F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32040" yWindow="1800" windowWidth="20310" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8445" yWindow="2070" windowWidth="20310" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,9 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AH3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Refactoring and Parameterizing of Give Feedback test auto assets
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0AD300-6519-409A-9D25-20D0A3DC15F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCEB375-1A9F-448D-8447-E1611E9DCC9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8445" yWindow="2070" windowWidth="20310" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -48,178 +48,181 @@
     <t>YE_Feedback_Knowledge</t>
   </si>
   <si>
+    <t>YE_Estimate</t>
+  </si>
+  <si>
+    <t>member for</t>
+  </si>
+  <si>
+    <t>Account_Membership_Term</t>
+  </si>
+  <si>
+    <t>YS_Tidiness</t>
+  </si>
+  <si>
+    <t>YS_Courtesy</t>
+  </si>
+  <si>
+    <t>YS_Reliability</t>
+  </si>
+  <si>
+    <t>YS_Workmanship</t>
+  </si>
+  <si>
+    <t>YS_Work_Description</t>
+  </si>
+  <si>
+    <t>New Test Toilet</t>
+  </si>
+  <si>
+    <t>YS_Work_Date</t>
+  </si>
+  <si>
+    <t>YS_Feedback_Published</t>
+  </si>
+  <si>
+    <t>Nice job</t>
+  </si>
+  <si>
+    <t>YD_Consumer_Customer</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>YD_Salutation</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>YD_Name</t>
+  </si>
+  <si>
+    <t>Ron Smith</t>
+  </si>
+  <si>
+    <t>YD_Postcode</t>
+  </si>
+  <si>
+    <t>YD_Verify_Address</t>
+  </si>
+  <si>
+    <t>YD_Best_Contact_Time</t>
+  </si>
+  <si>
+    <t>YD_Email</t>
+  </si>
+  <si>
+    <t>YD_Mobile</t>
+  </si>
+  <si>
+    <t>YD_Feedback_Method</t>
+  </si>
+  <si>
+    <t>YD_How_Did_You_Hear</t>
+  </si>
+  <si>
+    <t>YD_Reason_For_Tradeperson_Selection</t>
+  </si>
+  <si>
+    <t>YD_Receive_Chekatrade_Updates</t>
+  </si>
+  <si>
+    <t>YD_Receive_Third_Party_Updates</t>
+  </si>
+  <si>
+    <t>PO12 2SD</t>
+  </si>
+  <si>
+    <t>26 Broadsands Drive,Gosport,Hampshire,PO12:</t>
+  </si>
+  <si>
+    <t>Any Tme</t>
+  </si>
+  <si>
+    <t>burt_millichip@amail.com</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>YD_Company_Name</t>
+  </si>
+  <si>
+    <t>Testing Ltd</t>
+  </si>
+  <si>
+    <t>YD_Other_Response</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Had a dream</t>
+  </si>
+  <si>
+    <t>Prefer not to say</t>
+  </si>
+  <si>
+    <t>FD_Value_of_Work</t>
+  </si>
+  <si>
+    <t>FD_Verify_Sub_Header</t>
+  </si>
+  <si>
+    <t>FD_Verify_Button_Text</t>
+  </si>
+  <si>
+    <t>Value Of Work</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>FD_Sub_Text</t>
+  </si>
+  <si>
+    <t>Data Protection Act</t>
+  </si>
+  <si>
+    <t>FP_Sub_Header_Verify</t>
+  </si>
+  <si>
+    <t>FP_Sub_Text</t>
+  </si>
+  <si>
+    <t>FP_Button_Text</t>
+  </si>
+  <si>
+    <t>HP_Header_Verification</t>
+  </si>
+  <si>
+    <t>HP_Member_Link_Text_Verification</t>
+  </si>
+  <si>
+    <t>Thank you!</t>
+  </si>
+  <si>
+    <t>A Checkatrade staff member will now review</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Helping you find the right trade or service</t>
+  </si>
+  <si>
+    <t>or look up a member by name</t>
+  </si>
+  <si>
     <t>Agreed_price</t>
   </si>
   <si>
-    <t>YE_Estimate</t>
-  </si>
-  <si>
-    <t>member for</t>
-  </si>
-  <si>
-    <t>Account_Membership_Term</t>
-  </si>
-  <si>
-    <t>YS_Tidiness</t>
-  </si>
-  <si>
-    <t>YS_Courtesy</t>
-  </si>
-  <si>
-    <t>YS_Reliability</t>
-  </si>
-  <si>
-    <t>YS_Workmanship</t>
-  </si>
-  <si>
-    <t>YS_Work_Description</t>
-  </si>
-  <si>
-    <t>New Test Toilet</t>
-  </si>
-  <si>
-    <t>YS_Work_Date</t>
-  </si>
-  <si>
-    <t>YS_Days_to_CompleteYS_Work_Comments</t>
-  </si>
-  <si>
-    <t>YS_Feedback_Published</t>
-  </si>
-  <si>
-    <t>Nice job</t>
-  </si>
-  <si>
-    <t>YD_Consumer_Customer</t>
-  </si>
-  <si>
-    <t>Consumer</t>
-  </si>
-  <si>
-    <t>YD_Salutation</t>
-  </si>
-  <si>
-    <t>Mr</t>
-  </si>
-  <si>
-    <t>YD_Name</t>
-  </si>
-  <si>
-    <t>Ron Smith</t>
-  </si>
-  <si>
-    <t>YD_Postcode</t>
-  </si>
-  <si>
-    <t>YD_Verify_Address</t>
-  </si>
-  <si>
-    <t>YD_Best_Contact_Time</t>
-  </si>
-  <si>
-    <t>YD_Email</t>
-  </si>
-  <si>
-    <t>YD_Mobile</t>
-  </si>
-  <si>
-    <t>YD_Feedback_Method</t>
-  </si>
-  <si>
-    <t>YD_How_Did_You_Hear</t>
-  </si>
-  <si>
-    <t>YD_Reason_For_Tradeperson_Selection</t>
-  </si>
-  <si>
-    <t>YD_Receive_Chekatrade_Updates</t>
-  </si>
-  <si>
-    <t>YD_Receive_Third_Party_Updates</t>
-  </si>
-  <si>
-    <t>PO12 2SD</t>
-  </si>
-  <si>
-    <t>26 Broadsands Drive,Gosport,Hampshire,PO12:</t>
-  </si>
-  <si>
-    <t>Any Tme</t>
-  </si>
-  <si>
-    <t>burt_millichip@amail.com</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>YD_Company_Name</t>
-  </si>
-  <si>
-    <t>Testing Ltd</t>
-  </si>
-  <si>
-    <t>YD_Other_Response</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
-    <t>Had a dream</t>
-  </si>
-  <si>
-    <t>Prefer not to say</t>
-  </si>
-  <si>
-    <t>FD_Value_of_Work</t>
-  </si>
-  <si>
-    <t>FD_Verify_Sub_Header</t>
-  </si>
-  <si>
-    <t>FD_Verify_Button_Text</t>
-  </si>
-  <si>
-    <t>Value Of Work</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
-    <t>FD_Sub_Text</t>
-  </si>
-  <si>
-    <t>Data Protection Act</t>
-  </si>
-  <si>
-    <t>FP_Sub_Header_Verify</t>
-  </si>
-  <si>
-    <t>FP_Sub_Text</t>
-  </si>
-  <si>
-    <t>FP_Button_Text</t>
-  </si>
-  <si>
-    <t>HP_Header_Verification</t>
-  </si>
-  <si>
-    <t>HP_Member_Link_Text_Verification</t>
-  </si>
-  <si>
-    <t>Thank you!</t>
-  </si>
-  <si>
-    <t>A Checkatrade staff member will now review</t>
-  </si>
-  <si>
-    <t>Finish</t>
-  </si>
-  <si>
-    <t>Helping you find the right trade or service</t>
-  </si>
-  <si>
-    <t>or look up a member by name</t>
+    <t>YS_Days_to_Complete</t>
+  </si>
+  <si>
+    <t>YS_Work_Comments</t>
   </si>
 </sst>
 </file>
@@ -284,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -292,6 +295,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -575,7 +583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -583,7 +593,7 @@
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="7" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
@@ -591,7 +601,7 @@
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="43" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="22.5703125" customWidth="1"/>
     <col min="16" max="16" width="22.85546875" customWidth="1"/>
@@ -627,112 +637,115 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="AE1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="AH1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -743,13 +756,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="E2" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -767,55 +780,55 @@
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" s="3">
         <v>3</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O2" t="s">
         <v>5</v>
       </c>
       <c r="P2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>24</v>
       </c>
-      <c r="R2" t="s">
-        <v>26</v>
-      </c>
       <c r="S2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="T2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
         <v>37</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="V2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="X2">
         <v>7788123456</v>
       </c>
       <c r="Y2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" t="s">
         <v>45</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>47</v>
       </c>
       <c r="AC2" t="s">
         <v>5</v>
@@ -827,28 +840,28 @@
         <v>10000</v>
       </c>
       <c r="AF2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AG2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH2" t="s">
         <v>52</v>
       </c>
-      <c r="AH2" t="s">
-        <v>54</v>
-      </c>
       <c r="AI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" t="s">
         <v>60</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>61</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
         <v>62</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring and parameterizing Feedback function
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCEB375-1A9F-448D-8447-E1611E9DCC9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6787DC-44EC-4E30-A689-61FB2D65FF8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -135,15 +135,9 @@
     <t>PO12 2SD</t>
   </si>
   <si>
-    <t>26 Broadsands Drive,Gosport,Hampshire,PO12:</t>
-  </si>
-  <si>
     <t>Any Tme</t>
   </si>
   <si>
-    <t>burt_millichip@amail.com</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -223,6 +217,21 @@
   </si>
   <si>
     <t>YS_Work_Comments</t>
+  </si>
+  <si>
+    <t>YD_Home_Phone</t>
+  </si>
+  <si>
+    <t>Test_xxxxxx@xdxdxdxd.com</t>
+  </si>
+  <si>
+    <t>02392123456</t>
+  </si>
+  <si>
+    <t>07788123456</t>
+  </si>
+  <si>
+    <t>26 Broadsands Drive,Gosport,Hampshire,PO12 2SD</t>
   </si>
 </sst>
 </file>
@@ -581,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +610,7 @@
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" customWidth="1"/>
-    <col min="13" max="13" width="43" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="22.5703125" customWidth="1"/>
     <col min="16" max="16" width="22.85546875" customWidth="1"/>
@@ -609,27 +618,28 @@
     <col min="18" max="18" width="10.7109375" customWidth="1"/>
     <col min="19" max="19" width="19.140625" customWidth="1"/>
     <col min="20" max="20" width="13.42578125" customWidth="1"/>
-    <col min="21" max="21" width="43.42578125" customWidth="1"/>
-    <col min="22" max="22" width="21.28515625" customWidth="1"/>
-    <col min="23" max="23" width="25" customWidth="1"/>
-    <col min="24" max="24" width="13.85546875" customWidth="1"/>
-    <col min="25" max="25" width="21.85546875" customWidth="1"/>
-    <col min="26" max="27" width="22.140625" customWidth="1"/>
-    <col min="28" max="28" width="36.5703125" customWidth="1"/>
-    <col min="29" max="29" width="30.85546875" customWidth="1"/>
-    <col min="30" max="30" width="31" customWidth="1"/>
-    <col min="31" max="31" width="18.5703125" customWidth="1"/>
-    <col min="32" max="32" width="22.140625" customWidth="1"/>
-    <col min="33" max="33" width="21.5703125" customWidth="1"/>
-    <col min="34" max="34" width="18" customWidth="1"/>
-    <col min="35" max="35" width="29.28515625" customWidth="1"/>
-    <col min="36" max="36" width="34.140625" customWidth="1"/>
-    <col min="37" max="37" width="17.28515625" customWidth="1"/>
-    <col min="38" max="38" width="37.7109375" customWidth="1"/>
-    <col min="39" max="39" width="35.5703125" customWidth="1"/>
+    <col min="21" max="21" width="18" style="7" customWidth="1"/>
+    <col min="22" max="22" width="47.140625" customWidth="1"/>
+    <col min="23" max="23" width="21.28515625" customWidth="1"/>
+    <col min="24" max="24" width="25" customWidth="1"/>
+    <col min="25" max="25" width="13.85546875" style="7" customWidth="1"/>
+    <col min="26" max="26" width="21.85546875" customWidth="1"/>
+    <col min="27" max="28" width="22.140625" customWidth="1"/>
+    <col min="29" max="29" width="36.5703125" customWidth="1"/>
+    <col min="30" max="30" width="30.85546875" customWidth="1"/>
+    <col min="31" max="31" width="31" customWidth="1"/>
+    <col min="32" max="32" width="18.5703125" customWidth="1"/>
+    <col min="33" max="33" width="22.140625" customWidth="1"/>
+    <col min="34" max="34" width="21.5703125" customWidth="1"/>
+    <col min="35" max="35" width="18" customWidth="1"/>
+    <col min="36" max="36" width="29.28515625" customWidth="1"/>
+    <col min="37" max="37" width="34.140625" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" customWidth="1"/>
+    <col min="39" max="39" width="37.7109375" customWidth="1"/>
+    <col min="40" max="40" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -667,10 +677,10 @@
         <v>16</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>17</v>
@@ -685,70 +695,73 @@
         <v>23</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="AB1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -762,7 +775,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -801,72 +814,75 @@
         <v>24</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="T2" t="s">
         <v>35</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" t="s">
         <v>36</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z2" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="X2">
-        <v>7788123456</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
         <v>43</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>5</v>
       </c>
       <c r="AD2" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AE2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF2" s="3">
         <v>10000</v>
       </c>
-      <c r="AF2" t="s">
-        <v>49</v>
-      </c>
       <c r="AG2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI2" t="s">
         <v>50</v>
       </c>
-      <c r="AH2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL2" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AM2" t="s">
         <v>59</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AN2" t="s">
         <v>60</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W2" r:id="rId1" xr:uid="{2704FD4B-CF14-4148-BC2D-3E290DE31A7D}"/>
+    <hyperlink ref="X2" r:id="rId1" xr:uid="{2704FD4B-CF14-4148-BC2D-3E290DE31A7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Sunny day success, full E2E working OK, start of Give Feedback Validation Tests
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6787DC-44EC-4E30-A689-61FB2D65FF8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35765ED6-AB00-4836-B6E6-27F7422A1E67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
First stage of unattended testing phase
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35765ED6-AB00-4836-B6E6-27F7422A1E67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92C6775-DA46-4371-B31F-835C6EA53DEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working on Give Feedback, iteration of different option selections
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92C6775-DA46-4371-B31F-835C6EA53DEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D13C2DA-C30E-40A3-973F-BBD34BB38399}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="1305" windowWidth="48015" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -232,6 +232,36 @@
   </si>
   <si>
     <t>26 Broadsands Drive,Gosport,Hampshire,PO12 2SD</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>YE_Work_Carried_Out</t>
+  </si>
+  <si>
+    <t>YE_Nature_Of_Issue</t>
+  </si>
+  <si>
+    <t>YE_Comments</t>
+  </si>
+  <si>
+    <t>YE_Feedback_Published</t>
+  </si>
+  <si>
+    <t>YE_Reason_No_Feedback</t>
+  </si>
+  <si>
+    <t>No work carried out</t>
+  </si>
+  <si>
+    <t>Didn't want too</t>
+  </si>
+  <si>
+    <t>Test comment</t>
+  </si>
+  <si>
+    <t>YE_Resolve</t>
   </si>
 </sst>
 </file>
@@ -590,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AT32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,45 +631,46 @@
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" customWidth="1"/>
-    <col min="21" max="21" width="18" style="7" customWidth="1"/>
-    <col min="22" max="22" width="47.140625" customWidth="1"/>
-    <col min="23" max="23" width="21.28515625" customWidth="1"/>
-    <col min="24" max="24" width="25" customWidth="1"/>
-    <col min="25" max="25" width="13.85546875" style="7" customWidth="1"/>
-    <col min="26" max="26" width="21.85546875" customWidth="1"/>
-    <col min="27" max="28" width="22.140625" customWidth="1"/>
-    <col min="29" max="29" width="36.5703125" customWidth="1"/>
-    <col min="30" max="30" width="30.85546875" customWidth="1"/>
-    <col min="31" max="31" width="31" customWidth="1"/>
-    <col min="32" max="32" width="18.5703125" customWidth="1"/>
-    <col min="33" max="33" width="22.140625" customWidth="1"/>
-    <col min="34" max="34" width="21.5703125" customWidth="1"/>
-    <col min="35" max="35" width="18" customWidth="1"/>
-    <col min="36" max="36" width="29.28515625" customWidth="1"/>
-    <col min="37" max="37" width="34.140625" customWidth="1"/>
-    <col min="38" max="38" width="17.28515625" customWidth="1"/>
-    <col min="39" max="39" width="37.7109375" customWidth="1"/>
-    <col min="40" max="40" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="5" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="11" width="18.5703125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" customWidth="1"/>
+    <col min="20" max="20" width="19" customWidth="1"/>
+    <col min="21" max="21" width="22.5703125" customWidth="1"/>
+    <col min="22" max="22" width="22.85546875" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="19.140625" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" customWidth="1"/>
+    <col min="27" max="27" width="18" style="7" customWidth="1"/>
+    <col min="28" max="28" width="47.140625" customWidth="1"/>
+    <col min="29" max="29" width="21.28515625" customWidth="1"/>
+    <col min="30" max="30" width="25" customWidth="1"/>
+    <col min="31" max="31" width="13.85546875" style="7" customWidth="1"/>
+    <col min="32" max="32" width="21.85546875" customWidth="1"/>
+    <col min="33" max="34" width="22.140625" customWidth="1"/>
+    <col min="35" max="35" width="36.5703125" customWidth="1"/>
+    <col min="36" max="36" width="30.85546875" customWidth="1"/>
+    <col min="37" max="37" width="31" customWidth="1"/>
+    <col min="38" max="38" width="18.5703125" customWidth="1"/>
+    <col min="39" max="39" width="22.140625" customWidth="1"/>
+    <col min="40" max="40" width="21.5703125" customWidth="1"/>
+    <col min="41" max="41" width="18" customWidth="1"/>
+    <col min="42" max="42" width="29.28515625" customWidth="1"/>
+    <col min="43" max="43" width="34.140625" customWidth="1"/>
+    <col min="44" max="44" width="17.28515625" customWidth="1"/>
+    <col min="45" max="45" width="37.7109375" customWidth="1"/>
+    <col min="46" max="46" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -652,116 +683,134 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -774,117 +823,412 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="M2" s="3">
         <v>10</v>
       </c>
-      <c r="H2" s="3">
+      <c r="N2" s="3">
         <v>10</v>
       </c>
-      <c r="I2" s="3">
+      <c r="O2" s="3">
         <v>10</v>
       </c>
-      <c r="J2" s="3">
+      <c r="P2" s="3">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="3">
+      <c r="S2" s="3">
         <v>3</v>
       </c>
-      <c r="N2" t="s">
+      <c r="T2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" t="s">
+      <c r="U2" t="s">
         <v>5</v>
       </c>
-      <c r="P2" t="s">
+      <c r="V2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>22</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>24</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>39</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Z2" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
         <v>68</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AC2" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AF2" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AG2" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AH2" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AI2" t="s">
         <v>43</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AJ2" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AK2" t="s">
         <v>5</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AL2" s="3">
         <v>10000</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AM2" t="s">
         <v>47</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AN2" t="s">
         <v>48</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AO2" t="s">
         <v>50</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AP2" t="s">
         <v>56</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AQ2" t="s">
         <v>57</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AR2" t="s">
         <v>58</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AS2" t="s">
         <v>59</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AT2" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL3" s="3">
+        <v>10000</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="X2" r:id="rId1" xr:uid="{2704FD4B-CF14-4148-BC2D-3E290DE31A7D}"/>
+    <hyperlink ref="AD2" r:id="rId1" xr:uid="{2704FD4B-CF14-4148-BC2D-3E290DE31A7D}"/>
+    <hyperlink ref="AD3" r:id="rId2" xr:uid="{093AE99E-03C1-4040-B89F-8A01266ACA70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completion of 5 E2E Give Feedback Scenarios
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7867D3CF-9715-4FFC-A455-7EB2E042F01C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652FE365-FE1F-42D7-8CC6-D5016B198CA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="1590" windowWidth="49785" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6390" yWindow="3810" windowWidth="49455" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="106">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -237,58 +237,112 @@
     <t>No</t>
   </si>
   <si>
+    <t>Any Tme</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Prefer not to say</t>
+  </si>
+  <si>
+    <t>YS_Tidiness_ALT</t>
+  </si>
+  <si>
+    <t>YS_Reliability_ALT</t>
+  </si>
+  <si>
+    <t>YS_Courtesy_ALT</t>
+  </si>
+  <si>
+    <t>YS_Workmanship_ALT</t>
+  </si>
+  <si>
+    <t>YS_Work_Covered_ALT</t>
+  </si>
+  <si>
+    <t>YS_Discussed_Complaint_ALT</t>
+  </si>
+  <si>
+    <t>YS_Complaint_Reponse_ALT</t>
+  </si>
+  <si>
+    <t>It was my Cats fault</t>
+  </si>
+  <si>
+    <t>Parrot had a new Beak fitted</t>
+  </si>
+  <si>
+    <t>Parrot had to wait so long for a new beak?</t>
+  </si>
+  <si>
+    <t>Overcharging</t>
+  </si>
+  <si>
+    <t>Another Test comment</t>
+  </si>
+  <si>
+    <t>I would prefer not say</t>
+  </si>
+  <si>
+    <t>Agreed_price</t>
+  </si>
+  <si>
+    <t>New Test Toilet</t>
+  </si>
+  <si>
+    <t>Nice job</t>
+  </si>
+  <si>
+    <t>More_than_agreed_price_informed</t>
+  </si>
+  <si>
+    <t>New Parrot Fitted :-)</t>
+  </si>
+  <si>
+    <t>Call the Police</t>
+  </si>
+  <si>
+    <t>Between Midnight and 2AM</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Directed to Checkatrade</t>
+  </si>
+  <si>
+    <t>No work carried out</t>
+  </si>
+  <si>
     <t>Test comment</t>
   </si>
   <si>
-    <t>Any Tme</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
-    <t>Prefer not to say</t>
-  </si>
-  <si>
-    <t>YS_Tidiness_ALT</t>
-  </si>
-  <si>
-    <t>YS_Reliability_ALT</t>
-  </si>
-  <si>
-    <t>YS_Courtesy_ALT</t>
-  </si>
-  <si>
-    <t>YS_Workmanship_ALT</t>
-  </si>
-  <si>
-    <t>YS_Work_Covered_ALT</t>
-  </si>
-  <si>
-    <t>YS_Discussed_Complaint_ALT</t>
-  </si>
-  <si>
-    <t>YS_Complaint_Reponse_ALT</t>
-  </si>
-  <si>
-    <t>Tidiness</t>
+    <t>Didn't want too</t>
+  </si>
+  <si>
+    <t>After 6PM</t>
+  </si>
+  <si>
+    <t>Order Disagreement</t>
   </si>
   <si>
     <t>No Reason</t>
   </si>
   <si>
-    <t>A little bit untidy (score 5)</t>
-  </si>
-  <si>
-    <t>They worked around my timing (score 8)</t>
-  </si>
-  <si>
-    <t>Rude (score 3)</t>
-  </si>
-  <si>
-    <t>Excellent workmanship (score 10)</t>
-  </si>
-  <si>
     <t>It was my Grannies fault</t>
+  </si>
+  <si>
+    <t>Parrot had a new right leg fitted</t>
+  </si>
+  <si>
+    <t>Parrot had to wait so long for a new leg?</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t>Morning</t>
   </si>
 </sst>
 </file>
@@ -647,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:BA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,26 +712,27 @@
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="7" width="21.28515625" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="23" customWidth="1"/>
-    <col min="13" max="13" width="38.5703125" customWidth="1"/>
-    <col min="14" max="14" width="23" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
     <col min="15" max="15" width="18.5703125" customWidth="1"/>
-    <col min="16" max="17" width="23" customWidth="1"/>
+    <col min="16" max="16" width="21.85546875" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
     <col min="18" max="19" width="28.28515625" customWidth="1"/>
     <col min="20" max="20" width="12.5703125" customWidth="1"/>
     <col min="21" max="21" width="14.42578125" customWidth="1"/>
     <col min="22" max="22" width="13" customWidth="1"/>
     <col min="23" max="23" width="17.140625" customWidth="1"/>
-    <col min="24" max="24" width="19.5703125" customWidth="1"/>
+    <col min="24" max="24" width="32" customWidth="1"/>
     <col min="25" max="25" width="19.28515625" customWidth="1"/>
     <col min="26" max="26" width="22.28515625" customWidth="1"/>
-    <col min="27" max="27" width="19" customWidth="1"/>
+    <col min="27" max="27" width="30.7109375" customWidth="1"/>
     <col min="28" max="28" width="22.5703125" customWidth="1"/>
     <col min="29" max="29" width="22.85546875" customWidth="1"/>
     <col min="30" max="30" width="13.140625" customWidth="1"/>
@@ -743,25 +798,25 @@
         <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>10</v>
@@ -877,58 +932,38 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" t="s">
-        <v>83</v>
-      </c>
-      <c r="N2" t="s">
-        <v>84</v>
-      </c>
-      <c r="O2" t="s">
-        <v>85</v>
-      </c>
-      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="3">
+        <v>10</v>
+      </c>
+      <c r="U2" s="3">
+        <v>10</v>
+      </c>
+      <c r="V2" s="3">
+        <v>10</v>
+      </c>
+      <c r="W2" s="3">
+        <v>10</v>
+      </c>
+      <c r="X2" t="s">
         <v>87</v>
       </c>
-      <c r="T2" s="3">
-        <v>0</v>
-      </c>
-      <c r="U2" s="3">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3">
-        <v>0</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0</v>
+      <c r="Z2" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>5</v>
       </c>
       <c r="AC2" t="s">
         <v>18</v>
@@ -952,7 +987,7 @@
         <v>62</v>
       </c>
       <c r="AJ2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AK2" s="4" t="s">
         <v>59</v>
@@ -964,13 +999,13 @@
         <v>34</v>
       </c>
       <c r="AN2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO2" t="s">
         <v>38</v>
       </c>
       <c r="AP2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AQ2" t="s">
         <v>5</v>
@@ -979,7 +1014,7 @@
         <v>5</v>
       </c>
       <c r="AS2" s="3">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="AT2" t="s">
         <v>42</v>
@@ -1003,15 +1038,556 @@
         <v>54</v>
       </c>
       <c r="BA2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" s="3">
+        <v>2</v>
+      </c>
+      <c r="U3" s="3">
+        <v>3</v>
+      </c>
+      <c r="V3" s="3">
+        <v>3</v>
+      </c>
+      <c r="W3" s="3">
+        <v>1</v>
+      </c>
+      <c r="X3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>27</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS3" s="3">
+        <v>6789.99</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>97</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS4" s="3">
+        <v>10</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="3">
+        <v>5</v>
+      </c>
+      <c r="N5" s="3">
+        <v>8</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+      <c r="P5" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" t="s">
+        <v>101</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>157</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS5" s="3">
+        <v>20</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3">
+        <v>6</v>
+      </c>
+      <c r="N6" s="3">
+        <v>2</v>
+      </c>
+      <c r="O6" s="3">
+        <v>5</v>
+      </c>
+      <c r="P6" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" t="s">
+        <v>80</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>77</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS6" s="3">
+        <v>30</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA6" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AK2" r:id="rId1" xr:uid="{30845BF5-BD77-46BB-BD96-F5F965208380}"/>
+    <hyperlink ref="AK2" r:id="rId1" xr:uid="{77692886-2C5F-4109-B66F-3C1BFF8C7275}"/>
+    <hyperlink ref="AK4" r:id="rId2" xr:uid="{66D1021C-CD96-4CDE-8E9C-0E51C45BA6A7}"/>
+    <hyperlink ref="AK3" r:id="rId3" xr:uid="{47B16901-9498-4AF0-8755-B8C548C15939}"/>
+    <hyperlink ref="AK5" r:id="rId4" xr:uid="{1ECF8113-3F1A-40F8-9D7B-C3A07D1B5787}"/>
+    <hyperlink ref="AK6" r:id="rId5" xr:uid="{D0F301DC-880C-49D2-9DAE-DC3EBB90AB93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1192,14 +1768,14 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CD0F30E-EFF5-454C-8FB6-162270E122F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Completion of Give Feedback, Checking Firefox executiot issues when running the master test suite 200819
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652FE365-FE1F-42D7-8CC6-D5016B198CA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC54F8EA-4501-4AA6-B53C-3D7E4A01E3E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="3810" windowWidth="49455" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="3435" windowWidth="49455" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="107">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>Morning</t>
+  </si>
+  <si>
+    <t>Yet another Test comment</t>
   </si>
 </sst>
 </file>
@@ -703,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,19 +1181,43 @@
         <v>69</v>
       </c>
       <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="M4" s="3">
+        <v>5</v>
+      </c>
+      <c r="N4" s="3">
+        <v>8</v>
+      </c>
+      <c r="O4" s="3">
+        <v>3</v>
+      </c>
+      <c r="P4" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="s">
         <v>69</v>
       </c>
-      <c r="I4" t="s">
-        <v>97</v>
+      <c r="R4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" t="s">
+        <v>101</v>
       </c>
       <c r="T4" s="3">
         <v>0</v>
@@ -1204,6 +1231,15 @@
       <c r="W4" s="3">
         <v>0</v>
       </c>
+      <c r="X4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>157</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>103</v>
+      </c>
       <c r="AC4" t="s">
         <v>18</v>
       </c>
@@ -1226,7 +1262,7 @@
         <v>62</v>
       </c>
       <c r="AJ4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="AK4" s="4" t="s">
         <v>59</v>
@@ -1250,10 +1286,10 @@
         <v>5</v>
       </c>
       <c r="AR4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="AS4" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AT4" t="s">
         <v>42</v>
@@ -1297,40 +1333,40 @@
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="M5" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N5" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="O5" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P5" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q5" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="R5" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="S5" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="T5" s="3">
         <v>0</v>
@@ -1345,13 +1381,13 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="Z5" s="3">
-        <v>157</v>
+        <v>77</v>
       </c>
       <c r="AA5" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="AC5" t="s">
         <v>18</v>
@@ -1375,7 +1411,7 @@
         <v>62</v>
       </c>
       <c r="AJ5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AK5" s="4" t="s">
         <v>59</v>
@@ -1396,13 +1432,13 @@
         <v>72</v>
       </c>
       <c r="AQ5" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="AR5" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="AS5" s="3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AT5" t="s">
         <v>42</v>
@@ -1443,43 +1479,19 @@
         <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>83</v>
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
         <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="3">
-        <v>6</v>
-      </c>
-      <c r="N6" s="3">
-        <v>2</v>
-      </c>
-      <c r="O6" s="3">
-        <v>5</v>
-      </c>
-      <c r="P6" s="3">
-        <v>5</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R6" t="s">
-        <v>5</v>
-      </c>
-      <c r="S6" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="T6" s="3">
         <v>0</v>
@@ -1493,15 +1505,6 @@
       <c r="W6" s="3">
         <v>0</v>
       </c>
-      <c r="X6" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>77</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>82</v>
-      </c>
       <c r="AC6" t="s">
         <v>18</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>62</v>
       </c>
       <c r="AJ6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="AK6" s="4" t="s">
         <v>59</v>
@@ -1545,13 +1548,13 @@
         <v>72</v>
       </c>
       <c r="AQ6" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="AR6" t="s">
         <v>5</v>
       </c>
       <c r="AS6" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="AT6" t="s">
         <v>42</v>
@@ -1581,10 +1584,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AK2" r:id="rId1" xr:uid="{77692886-2C5F-4109-B66F-3C1BFF8C7275}"/>
-    <hyperlink ref="AK4" r:id="rId2" xr:uid="{66D1021C-CD96-4CDE-8E9C-0E51C45BA6A7}"/>
+    <hyperlink ref="AK6" r:id="rId2" xr:uid="{66D1021C-CD96-4CDE-8E9C-0E51C45BA6A7}"/>
     <hyperlink ref="AK3" r:id="rId3" xr:uid="{47B16901-9498-4AF0-8755-B8C548C15939}"/>
-    <hyperlink ref="AK5" r:id="rId4" xr:uid="{1ECF8113-3F1A-40F8-9D7B-C3A07D1B5787}"/>
-    <hyperlink ref="AK6" r:id="rId5" xr:uid="{D0F301DC-880C-49D2-9DAE-DC3EBB90AB93}"/>
+    <hyperlink ref="AK4" r:id="rId4" xr:uid="{1ECF8113-3F1A-40F8-9D7B-C3A07D1B5787}"/>
+    <hyperlink ref="AK5" r:id="rId5" xr:uid="{D0F301DC-880C-49D2-9DAE-DC3EBB90AB93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -1592,6 +1595,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003D03B8ECFDD40043937B6ECC33B46815" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="84137c46b2a6eace2e7af72d8f77c98b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="832d7cee4ce45ac774980f8322b40d1a" ns3:_="">
     <xsd:import namespace="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
@@ -1723,22 +1741,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CD0F30E-EFF5-454C-8FB6-162270E122F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07FD2A87-FF1D-4387-80BE-6E5019E04D37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8168A49-8272-495A-9410-56E44D363D7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1754,28 +1781,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07FD2A87-FF1D-4387-80BE-6E5019E04D37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CD0F30E-EFF5-454C-8FB6-162270E122F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to Give Feedback tests primarily
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\git\src\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC54F8EA-4501-4AA6-B53C-3D7E4A01E3E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A17A876-453F-450E-8917-7D11F73176C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="3435" windowWidth="49455" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3645" yWindow="3390" windowWidth="20940" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="113">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -346,6 +346,24 @@
   </si>
   <si>
     <t>Yet another Test comment</t>
+  </si>
+  <si>
+    <t>YE_Other_Trade</t>
+  </si>
+  <si>
+    <t>YE_Other_Trade_Selection</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -704,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA6"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,55 +733,55 @@
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" customWidth="1"/>
-    <col min="16" max="16" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="23" customWidth="1"/>
-    <col min="18" max="19" width="28.28515625" customWidth="1"/>
-    <col min="20" max="20" width="12.5703125" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" customWidth="1"/>
-    <col min="22" max="22" width="13" customWidth="1"/>
-    <col min="23" max="23" width="17.140625" customWidth="1"/>
-    <col min="24" max="24" width="32" customWidth="1"/>
-    <col min="25" max="25" width="19.28515625" customWidth="1"/>
-    <col min="26" max="26" width="22.28515625" customWidth="1"/>
-    <col min="27" max="27" width="30.7109375" customWidth="1"/>
-    <col min="28" max="28" width="22.5703125" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" customWidth="1"/>
-    <col min="32" max="32" width="19.140625" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" customWidth="1"/>
-    <col min="34" max="34" width="18" style="7" customWidth="1"/>
-    <col min="35" max="35" width="47.140625" customWidth="1"/>
-    <col min="36" max="36" width="24.5703125" customWidth="1"/>
-    <col min="37" max="37" width="25" customWidth="1"/>
-    <col min="38" max="38" width="13.85546875" style="7" customWidth="1"/>
-    <col min="39" max="39" width="21.85546875" customWidth="1"/>
-    <col min="40" max="41" width="22.140625" customWidth="1"/>
-    <col min="42" max="42" width="43.7109375" customWidth="1"/>
-    <col min="43" max="43" width="30.85546875" customWidth="1"/>
-    <col min="44" max="44" width="31" customWidth="1"/>
-    <col min="45" max="45" width="18.5703125" customWidth="1"/>
-    <col min="46" max="46" width="22.140625" customWidth="1"/>
-    <col min="47" max="47" width="21.5703125" customWidth="1"/>
-    <col min="48" max="48" width="18" customWidth="1"/>
-    <col min="49" max="49" width="29.28515625" customWidth="1"/>
-    <col min="50" max="50" width="34.140625" customWidth="1"/>
-    <col min="51" max="51" width="17.28515625" customWidth="1"/>
-    <col min="52" max="52" width="37.7109375" customWidth="1"/>
-    <col min="53" max="53" width="35.5703125" customWidth="1"/>
+    <col min="4" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="7" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" customWidth="1"/>
+    <col min="19" max="19" width="23" customWidth="1"/>
+    <col min="20" max="21" width="28.28515625" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" customWidth="1"/>
+    <col min="24" max="24" width="13" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" customWidth="1"/>
+    <col min="26" max="26" width="32" customWidth="1"/>
+    <col min="27" max="27" width="19.28515625" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" customWidth="1"/>
+    <col min="29" max="29" width="30.7109375" customWidth="1"/>
+    <col min="30" max="30" width="22.5703125" customWidth="1"/>
+    <col min="31" max="31" width="22.85546875" customWidth="1"/>
+    <col min="32" max="32" width="13.140625" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" customWidth="1"/>
+    <col min="34" max="34" width="19.140625" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" customWidth="1"/>
+    <col min="36" max="36" width="18" style="7" customWidth="1"/>
+    <col min="37" max="37" width="47.140625" customWidth="1"/>
+    <col min="38" max="38" width="24.5703125" customWidth="1"/>
+    <col min="39" max="39" width="25" customWidth="1"/>
+    <col min="40" max="40" width="13.85546875" style="7" customWidth="1"/>
+    <col min="41" max="41" width="21.85546875" customWidth="1"/>
+    <col min="42" max="43" width="22.140625" customWidth="1"/>
+    <col min="44" max="44" width="43.7109375" customWidth="1"/>
+    <col min="45" max="45" width="30.85546875" customWidth="1"/>
+    <col min="46" max="46" width="31" customWidth="1"/>
+    <col min="47" max="47" width="18.5703125" customWidth="1"/>
+    <col min="48" max="48" width="22.140625" customWidth="1"/>
+    <col min="49" max="49" width="21.5703125" customWidth="1"/>
+    <col min="50" max="50" width="18" customWidth="1"/>
+    <col min="51" max="51" width="29.28515625" customWidth="1"/>
+    <col min="52" max="52" width="34.140625" customWidth="1"/>
+    <col min="53" max="53" width="17.28515625" customWidth="1"/>
+    <col min="54" max="54" width="37.7109375" customWidth="1"/>
+    <col min="55" max="55" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -777,154 +795,160 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -937,18 +961,18 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7">
+        <v>11</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-      <c r="T2" s="3">
-        <v>10</v>
-      </c>
-      <c r="U2" s="3">
-        <v>10</v>
+      <c r="M2" s="6"/>
+      <c r="N2" t="s">
+        <v>5</v>
       </c>
       <c r="V2" s="3">
         <v>10</v>
@@ -956,95 +980,101 @@
       <c r="W2" s="3">
         <v>10</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="3">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>10</v>
+      </c>
+      <c r="Z2" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="AB2" s="3">
         <v>3</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>88</v>
       </c>
-      <c r="AB2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" t="s">
         <v>18</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>22</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>62</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
         <v>70</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AO2" t="s">
         <v>34</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>71</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>38</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AR2" t="s">
         <v>72</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS2" s="3">
+      <c r="AS2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU2" s="3">
         <v>10000</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AV2" t="s">
         <v>42</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AW2" t="s">
         <v>43</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AX2" t="s">
         <v>45</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AY2" t="s">
         <v>51</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AZ2" t="s">
         <v>52</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BA2" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BB2" t="s">
         <v>54</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BC2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1057,117 +1087,123 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" t="s">
+      <c r="M3" s="6"/>
+      <c r="N3" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="3">
+      <c r="V3" s="3">
         <v>2</v>
       </c>
-      <c r="U3" s="3">
+      <c r="W3" s="3">
         <v>3</v>
       </c>
-      <c r="V3" s="3">
+      <c r="X3" s="3">
         <v>3</v>
       </c>
-      <c r="W3" s="3">
+      <c r="Y3" s="3">
         <v>1</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>90</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AB3" s="3">
         <v>27</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>91</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>69</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
         <v>18</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AF3" t="s">
         <v>20</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>22</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>36</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AI3" t="s">
         <v>33</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AJ3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AK3" t="s">
         <v>62</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AL3" t="s">
         <v>92</v>
       </c>
-      <c r="AK3" s="4" t="s">
+      <c r="AM3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AL3" s="6" t="s">
+      <c r="AN3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AO3" t="s">
         <v>34</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AP3" t="s">
         <v>93</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AQ3" t="s">
         <v>38</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AR3" t="s">
         <v>94</v>
       </c>
-      <c r="AQ3" t="s">
+      <c r="AS3" t="s">
         <v>69</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AT3" t="s">
         <v>69</v>
       </c>
-      <c r="AS3" s="3">
+      <c r="AU3" s="3">
         <v>6789.99</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AV3" t="s">
         <v>42</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AW3" t="s">
         <v>43</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AX3" t="s">
         <v>45</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AY3" t="s">
         <v>51</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="AZ3" t="s">
         <v>52</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="BA3" t="s">
         <v>53</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BB3" t="s">
         <v>54</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BC3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1183,47 +1219,47 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>84</v>
       </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
         <v>100</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="3">
-        <v>5</v>
-      </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
+        <v>5</v>
+      </c>
+      <c r="P4" s="3">
         <v>8</v>
       </c>
-      <c r="O4" s="3">
+      <c r="Q4" s="3">
         <v>3</v>
       </c>
-      <c r="P4" s="3">
+      <c r="R4" s="3">
         <v>10</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>69</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>69</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>101</v>
-      </c>
-      <c r="T4" s="3">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3">
-        <v>0</v>
       </c>
       <c r="V4" s="3">
         <v>0</v>
@@ -1231,92 +1267,98 @@
       <c r="W4" s="3">
         <v>0</v>
       </c>
-      <c r="X4" t="s">
+      <c r="X4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
         <v>102</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AB4" s="3">
         <v>157</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AC4" t="s">
         <v>103</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
         <v>18</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AF4" t="s">
         <v>20</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>22</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>36</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AI4" t="s">
         <v>33</v>
       </c>
-      <c r="AH4" s="6" t="s">
+      <c r="AJ4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AK4" t="s">
         <v>62</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AL4" t="s">
         <v>104</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AM4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AL4" s="6" t="s">
+      <c r="AN4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AO4" t="s">
         <v>34</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AP4" t="s">
         <v>71</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="AQ4" t="s">
         <v>38</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AR4" t="s">
         <v>72</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT4" t="s">
         <v>69</v>
       </c>
-      <c r="AS4" s="3">
+      <c r="AU4" s="3">
         <v>20</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AV4" t="s">
         <v>42</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AW4" t="s">
         <v>43</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AX4" t="s">
         <v>45</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="AY4" t="s">
         <v>51</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AZ4" t="s">
         <v>52</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BA4" t="s">
         <v>53</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BB4" t="s">
         <v>54</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BC4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1332,47 +1374,47 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>106</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>69</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="3">
+      <c r="M5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="3">
         <v>6</v>
       </c>
-      <c r="N5" s="3">
+      <c r="P5" s="3">
         <v>2</v>
       </c>
-      <c r="O5" s="3">
-        <v>5</v>
-      </c>
-      <c r="P5" s="3">
-        <v>5</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>5</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="Q5" s="3">
+        <v>5</v>
+      </c>
+      <c r="R5" s="3">
         <v>5</v>
       </c>
       <c r="S5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" t="s">
         <v>80</v>
-      </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
       </c>
       <c r="V5" s="3">
         <v>0</v>
@@ -1380,92 +1422,98 @@
       <c r="W5" s="3">
         <v>0</v>
       </c>
-      <c r="X5" t="s">
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
         <v>81</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="AB5" s="3">
         <v>77</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AC5" t="s">
         <v>82</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AE5" t="s">
         <v>18</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AF5" t="s">
         <v>20</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>22</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AH5" t="s">
         <v>36</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AI5" t="s">
         <v>33</v>
       </c>
-      <c r="AH5" s="6" t="s">
+      <c r="AJ5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AK5" t="s">
         <v>62</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AL5" t="s">
         <v>105</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AM5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AL5" s="6" t="s">
+      <c r="AN5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AO5" t="s">
         <v>34</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AP5" t="s">
         <v>71</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AQ5" t="s">
         <v>38</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AR5" t="s">
         <v>72</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AS5" t="s">
         <v>69</v>
       </c>
-      <c r="AR5" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS5" s="3">
+      <c r="AT5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU5" s="3">
         <v>30</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AV5" t="s">
         <v>42</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AW5" t="s">
         <v>43</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AX5" t="s">
         <v>45</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AY5" t="s">
         <v>51</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AZ5" t="s">
         <v>52</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="BA5" t="s">
         <v>53</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BB5" t="s">
         <v>54</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BC5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1479,25 +1527,25 @@
         <v>69</v>
       </c>
       <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
         <v>69</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>95</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>96</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>69</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>97</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0</v>
       </c>
       <c r="V6" s="3">
         <v>0</v>
@@ -1505,89 +1553,95 @@
       <c r="W6" s="3">
         <v>0</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="s">
         <v>18</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AF6" t="s">
         <v>20</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>22</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>36</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AI6" t="s">
         <v>33</v>
       </c>
-      <c r="AH6" s="6" t="s">
+      <c r="AJ6" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AK6" t="s">
         <v>62</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AL6" t="s">
         <v>98</v>
       </c>
-      <c r="AK6" s="4" t="s">
+      <c r="AM6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AL6" s="6" t="s">
+      <c r="AN6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AO6" t="s">
         <v>34</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AP6" t="s">
         <v>71</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AQ6" t="s">
         <v>38</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AR6" t="s">
         <v>72</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS6" s="3">
+      <c r="AS6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU6" s="3">
         <v>10</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AV6" t="s">
         <v>42</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AW6" t="s">
         <v>43</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AX6" t="s">
         <v>45</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AY6" t="s">
         <v>51</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AZ6" t="s">
         <v>52</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="BA6" t="s">
         <v>53</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="BB6" t="s">
         <v>54</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BC6" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AK2" r:id="rId1" xr:uid="{77692886-2C5F-4109-B66F-3C1BFF8C7275}"/>
-    <hyperlink ref="AK6" r:id="rId2" xr:uid="{66D1021C-CD96-4CDE-8E9C-0E51C45BA6A7}"/>
-    <hyperlink ref="AK3" r:id="rId3" xr:uid="{47B16901-9498-4AF0-8755-B8C548C15939}"/>
-    <hyperlink ref="AK4" r:id="rId4" xr:uid="{1ECF8113-3F1A-40F8-9D7B-C3A07D1B5787}"/>
-    <hyperlink ref="AK5" r:id="rId5" xr:uid="{D0F301DC-880C-49D2-9DAE-DC3EBB90AB93}"/>
+    <hyperlink ref="AM2" r:id="rId1" xr:uid="{77692886-2C5F-4109-B66F-3C1BFF8C7275}"/>
+    <hyperlink ref="AM6" r:id="rId2" xr:uid="{66D1021C-CD96-4CDE-8E9C-0E51C45BA6A7}"/>
+    <hyperlink ref="AM3" r:id="rId3" xr:uid="{47B16901-9498-4AF0-8755-B8C548C15939}"/>
+    <hyperlink ref="AM4" r:id="rId4" xr:uid="{1ECF8113-3F1A-40F8-9D7B-C3A07D1B5787}"/>
+    <hyperlink ref="AM5" r:id="rId5" xr:uid="{D0F301DC-880C-49D2-9DAE-DC3EBB90AB93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -1595,18 +1649,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1742,6 +1796,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07FD2A87-FF1D-4387-80BE-6E5019E04D37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CD0F30E-EFF5-454C-8FB6-162270E122F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1753,14 +1815,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07FD2A87-FF1D-4387-80BE-6E5019E04D37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Give Feedback Fixes factored into tests, plus added extra WO tests
</commit_message>
<xml_diff>
--- a/Data Files/Give_Feedback.xlsx
+++ b/Data Files/Give_Feedback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\git\src\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A17A876-453F-450E-8917-7D11F73176C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00146362-7F8F-4F6A-8E3F-ADDDA2A3925E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="3390" windowWidth="20940" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="112">
   <si>
     <t>Account_Verification_Name</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Selsey, Chichester, West Sussex</t>
-  </si>
-  <si>
-    <t>Test Account</t>
   </si>
   <si>
     <t>YE_Recommendations</t>
@@ -725,7 +722,7 @@
   <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,190 +786,190 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AO1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AT1" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="AU1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="AX1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AY1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="6">
+        <v>443671</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="7">
         <v>11</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V2" s="3">
         <v>10</v>
@@ -987,121 +984,121 @@
         <v>10</v>
       </c>
       <c r="Z2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB2" s="3">
         <v>3</v>
       </c>
       <c r="AC2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AF2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AG2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AH2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AI2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL2" t="s">
+      <c r="AP2" t="s">
         <v>70</v>
       </c>
-      <c r="AM2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR2" t="s">
         <v>71</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>72</v>
-      </c>
       <c r="AS2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU2" s="3">
         <v>10000</v>
       </c>
       <c r="AV2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW2" t="s">
         <v>42</v>
       </c>
-      <c r="AW2" t="s">
-        <v>43</v>
-      </c>
       <c r="AX2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>51</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" t="s">
         <v>52</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>53</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>54</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="6">
+        <v>443671</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V3" s="3">
         <v>2</v>
@@ -1116,129 +1113,129 @@
         <v>1</v>
       </c>
       <c r="Z3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AB3" s="3">
         <v>27</v>
       </c>
       <c r="AC3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL3" t="s">
         <v>91</v>
       </c>
-      <c r="AD3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI3" t="s">
+      <c r="AM3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL3" t="s">
+      <c r="AP3" t="s">
         <v>92</v>
       </c>
-      <c r="AM3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR3" t="s">
         <v>93</v>
       </c>
-      <c r="AQ3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>94</v>
-      </c>
       <c r="AS3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AT3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AU3" s="3">
         <v>6789.99</v>
       </c>
       <c r="AV3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW3" t="s">
         <v>42</v>
       </c>
-      <c r="AW3" t="s">
-        <v>43</v>
-      </c>
       <c r="AX3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ3" t="s">
         <v>51</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
         <v>52</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
         <v>53</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BC3" t="s">
         <v>54</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4" s="6">
+        <v>443671</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
         <v>99</v>
       </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" t="s">
-        <v>100</v>
-      </c>
       <c r="M4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O4" s="3">
         <v>5</v>
@@ -1253,13 +1250,13 @@
         <v>10</v>
       </c>
       <c r="S4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V4" s="3">
         <v>0</v>
@@ -1274,126 +1271,126 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB4" s="3">
         <v>157</v>
       </c>
       <c r="AC4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL4" t="s">
         <v>103</v>
       </c>
-      <c r="AE4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI4" t="s">
+      <c r="AM4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO4" t="s">
         <v>33</v>
       </c>
-      <c r="AJ4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>34</v>
-      </c>
       <c r="AP4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR4" t="s">
         <v>71</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>72</v>
-      </c>
       <c r="AS4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AU4" s="3">
         <v>20</v>
       </c>
       <c r="AV4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW4" t="s">
         <v>42</v>
       </c>
-      <c r="AW4" t="s">
-        <v>43</v>
-      </c>
       <c r="AX4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>51</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BA4" t="s">
         <v>52</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BB4" t="s">
         <v>53</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BC4" t="s">
         <v>54</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5" s="6">
+        <v>443671</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O5" s="3">
         <v>6</v>
@@ -1408,13 +1405,13 @@
         <v>5</v>
       </c>
       <c r="S5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V5" s="3">
         <v>0</v>
@@ -1429,123 +1426,123 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB5" s="3">
         <v>77</v>
       </c>
       <c r="AC5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AE5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AF5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AG5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AH5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AI5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO5" t="s">
         <v>33</v>
       </c>
-      <c r="AJ5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>34</v>
-      </c>
       <c r="AP5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR5" t="s">
         <v>71</v>
       </c>
-      <c r="AQ5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>72</v>
-      </c>
       <c r="AS5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AT5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU5" s="3">
         <v>30</v>
       </c>
       <c r="AV5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW5" t="s">
         <v>42</v>
       </c>
-      <c r="AW5" t="s">
-        <v>43</v>
-      </c>
       <c r="AX5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ5" t="s">
         <v>51</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BA5" t="s">
         <v>52</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BB5" t="s">
         <v>53</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BC5" t="s">
         <v>54</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
+      <c r="A6" s="6">
+        <v>443671</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" t="s">
         <v>95</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" t="s">
         <v>96</v>
-      </c>
-      <c r="J6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" t="s">
-        <v>97</v>
       </c>
       <c r="V6" s="3">
         <v>0</v>
@@ -1560,79 +1557,79 @@
         <v>0</v>
       </c>
       <c r="AE6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AF6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AG6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AH6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AI6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO6" t="s">
         <v>33</v>
       </c>
-      <c r="AJ6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>34</v>
-      </c>
       <c r="AP6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR6" t="s">
         <v>71</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>72</v>
-      </c>
       <c r="AS6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU6" s="3">
         <v>10</v>
       </c>
       <c r="AV6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW6" t="s">
         <v>42</v>
       </c>
-      <c r="AW6" t="s">
-        <v>43</v>
-      </c>
       <c r="AX6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ6" t="s">
         <v>51</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="BA6" t="s">
         <v>52</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BB6" t="s">
         <v>53</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BC6" t="s">
         <v>54</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1649,21 +1646,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003D03B8ECFDD40043937B6ECC33B46815" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="84137c46b2a6eace2e7af72d8f77c98b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="832d7cee4ce45ac774980f8322b40d1a" ns3:_="">
     <xsd:import namespace="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
@@ -1795,31 +1777,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07FD2A87-FF1D-4387-80BE-6E5019E04D37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CD0F30E-EFF5-454C-8FB6-162270E122F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8168A49-8272-495A-9410-56E44D363D7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1835,4 +1808,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07FD2A87-FF1D-4387-80BE-6E5019E04D37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CD0F30E-EFF5-454C-8FB6-162270E122F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3cc1c52b-567e-4ca0-9b0a-cdf6f73b4509"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>